<commit_message>
🚀 datos ya 3
</commit_message>
<xml_diff>
--- a/aplicaciones/www/estaticos/datos/descarga/ya3-1-saber11-matematicas.xlsx
+++ b/aplicaciones/www/estaticos/datos/descarga/ya3-1-saber11-matematicas.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28619"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_C3CEF80CD967B36491239BAE5E4E46ABFAFEF70B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_C3CEF80CD967B36491239BAE5E4E46ABFAFEF70B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF5923C3-CAB6-423C-BD76-483359B84DFE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="datos" sheetId="1" r:id="rId1"/>
+    <sheet name="metadatos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3961" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3974" uniqueCount="20">
   <si>
     <t>anno</t>
   </si>
@@ -65,18 +66,56 @@
   <si>
     <t>2023</t>
   </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Fuente</t>
+  </si>
+  <si>
+    <t>Fecha_de_extracción</t>
+  </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Código del municipio</t>
+  </si>
+  <si>
+    <t>Total de niñas y niños con educación inicial en el marco de la atención integral</t>
+  </si>
+  <si>
+    <t>DataIcfes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,8 +138,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,7 +440,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3960"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
@@ -43958,4 +44001,78 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6810E883-67EE-4205-8AEF-F82E2630899A}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45715</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45715</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45715</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>